<commit_message>
Committing so I can Update
</commit_message>
<xml_diff>
--- a/aws_coords_2017.xlsx
+++ b/aws_coords_2017.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\Desktop\Antarctica-Weather-Station-Intercative-Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katezellmer/Documents/Geo 575/Antarctica Weather Station/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10485" yWindow="465" windowWidth="23145" windowHeight="16260" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="5660" yWindow="460" windowWidth="23140" windowHeight="16260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2017_all" sheetId="1" r:id="rId1"/>
     <sheet name="q1h_aws" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1332,13 +1336,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B66" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.875" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3399,7 +3403,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>585</v>
       </c>
@@ -3419,7 +3423,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>572</v>
       </c>
@@ -3439,7 +3443,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>589</v>
       </c>
@@ -3459,7 +3463,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>588</v>
       </c>
@@ -3479,7 +3483,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>590</v>
       </c>
@@ -3499,7 +3503,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>440</v>
       </c>
@@ -3519,7 +3523,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>676</v>
       </c>
@@ -3539,7 +3543,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>623</v>
       </c>
@@ -3559,7 +3563,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>394</v>
       </c>
@@ -3579,7 +3583,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>344</v>
       </c>
@@ -3599,7 +3603,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>633</v>
       </c>
@@ -3619,7 +3623,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>667</v>
       </c>
@@ -3639,7 +3643,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>625</v>
       </c>
@@ -3659,7 +3663,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>632</v>
       </c>
@@ -3679,7 +3683,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>610</v>
       </c>
@@ -3699,7 +3703,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>627</v>
       </c>
@@ -3719,7 +3723,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>679</v>
       </c>
@@ -3739,7 +3743,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>635</v>
       </c>
@@ -3759,7 +3763,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>636</v>
       </c>
@@ -3779,7 +3783,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>629</v>
       </c>
@@ -3799,7 +3803,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>390</v>
       </c>
@@ -3819,7 +3823,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>638</v>
       </c>
@@ -3839,7 +3843,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>607</v>
       </c>
@@ -3859,7 +3863,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>401</v>
       </c>
@@ -3879,7 +3883,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>624</v>
       </c>
@@ -3899,7 +3903,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>608</v>
       </c>
@@ -3919,7 +3923,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>670</v>
       </c>
@@ -3939,7 +3943,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>397</v>
       </c>
@@ -3959,7 +3963,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>680</v>
       </c>
@@ -3979,7 +3983,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>673</v>
       </c>
@@ -3999,7 +4003,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>189</v>
       </c>
@@ -4019,7 +4023,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>665</v>
       </c>
@@ -4039,7 +4043,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>666</v>
       </c>
@@ -4059,7 +4063,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>630</v>
       </c>
@@ -4079,7 +4083,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>600</v>
       </c>
@@ -4099,7 +4103,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>669</v>
       </c>
@@ -4119,7 +4123,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>606</v>
       </c>
@@ -4139,7 +4143,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>674</v>
       </c>
@@ -4159,7 +4163,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>265</v>
       </c>
@@ -4179,7 +4183,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>441</v>
       </c>
@@ -4199,7 +4203,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>671</v>
       </c>
@@ -4219,7 +4223,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>640</v>
       </c>
@@ -4239,7 +4243,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>639</v>
       </c>
@@ -4259,7 +4263,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>634</v>
       </c>
@@ -4279,7 +4283,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>628</v>
       </c>
@@ -4299,7 +4303,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>668</v>
       </c>
@@ -4319,7 +4323,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>404</v>
       </c>
@@ -4339,7 +4343,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>672</v>
       </c>
@@ -4359,7 +4363,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>675</v>
       </c>
@@ -4379,7 +4383,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>389</v>
       </c>
@@ -4399,7 +4403,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>240</v>
       </c>
@@ -4419,7 +4423,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>678</v>
       </c>
@@ -4439,7 +4443,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>681</v>
       </c>
@@ -4459,7 +4463,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>677</v>
       </c>
@@ -4479,7 +4483,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>619</v>
       </c>
@@ -4499,7 +4503,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>648</v>
       </c>
@@ -4519,7 +4523,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>349</v>
       </c>
@@ -4539,7 +4543,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>132</v>
       </c>
@@ -4559,7 +4563,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>218</v>
       </c>
@@ -4579,7 +4583,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>376</v>
       </c>
@@ -4599,7 +4603,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>584</v>
       </c>
@@ -4619,7 +4623,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>576</v>
       </c>
@@ -4673,13 +4677,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.875" style="2"/>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6122,4 +6124,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>